<commit_message>
caricamento report checklist aggiornata
La report check list è stata aggiornata inserendo maggiori dettagli sulla gestione degli errori per i casi con ID [48, 152, 160, 163], su richiesta del team FSE con mail del 05/02/2024
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111#ITAMEDICALXX/Critex/Meditex/4/report-checklist.xlsx
+++ b/GATEWAY/A1#111#ITAMEDICALXX/Critex/Meditex/4/report-checklist.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\.shortcut-targets-by-id\0B3Vzr79vD6P9ZUVVMG5DUUh6MWc\MedITEX\FSE 2.0\Accreditamento\FILES ACCREDITAMENTO MEDITEX\risultati\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\.shortcut-targets-by-id\0B3Vzr79vD6P9ZUVVMG5DUUh6MWc\MedITEX\FSE 2.0\Accreditamento\FILES ACCREDITAMENTO MEDITEX\RSA\risultati\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F05FBA73-A8FE-44B6-B13B-EA307F940277}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FF0FF62-F195-4CAA-8453-776E4F88DA36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2172" uniqueCount="893">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2172" uniqueCount="894">
   <si>
     <t>COME VALORIZZARE LA CHECKLIST (tab TestCases)</t>
   </si>
@@ -4553,9 +4553,6 @@
 0100: ceId":"UNKNOWN_WORKFLOW_ID"}</t>
   </si>
   <si>
-    <t>In caso di timeout con il gateway il processo clinico prosegue, il referto viene prodotto. Il documento viene aggiunto alla lista dei messaggi inviati senza che venga evidenziato il corretto invio (Luce verde) o l'errato invio (luce rossa). Il messaggio può essere inviato in un secondo momento</t>
-  </si>
-  <si>
     <t>2024-01-23T09:37:58Z</t>
   </si>
   <si>
@@ -4636,6 +4633,12 @@
   </si>
   <si>
     <t>2.16.840.1.113883.2.9.2.120.4.4.f37c2e09307325d28ffebdd2d787c459ac067df7a7e84e065998e7776dc4a5af.a53e7bd7cc^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In caso di timeout con il gateway il processo clinico prosegue, il referto viene prodotto. Il documento viene aggiunto alla lista dei messaggi inviati senza che venga evidenziato il corretto invio (Luce verde) o la ricezione di un errore (luce rossa). L'applicativo inserisce il documento in una coda che si occupa di eseguire in automatico un nuovo tentativo di invio. </t>
+  </si>
+  <si>
+    <t>L'utente ha a disposizione la lista dei messaggi inviati. Per quelli non andati a buon fine viene segnalata la descrizione dell'errore. Una volta che l'errore è stato corretto il messaggio può essere nuovamente inviato da parte dell'utente.</t>
   </si>
 </sst>
 </file>
@@ -7565,10 +7568,10 @@
   <dimension ref="A1:T1000"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="G39" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="M55" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="I170" sqref="I170"/>
+      <selection pane="bottomRight" activeCell="P170" sqref="P170"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -8811,7 +8814,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="39" spans="1:20" ht="25.8" customHeight="1">
+    <row r="39" spans="1:20" ht="25.8" hidden="1" customHeight="1">
       <c r="A39" s="20">
         <v>32</v>
       </c>
@@ -9103,7 +9106,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="47" spans="1:20" ht="14.25" customHeight="1">
+    <row r="47" spans="1:20" ht="14.25" hidden="1" customHeight="1">
       <c r="A47" s="20">
         <v>40</v>
       </c>
@@ -9403,7 +9406,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="55" spans="1:20" ht="14.25" hidden="1" customHeight="1">
+    <row r="55" spans="1:20" ht="14.25" customHeight="1">
       <c r="A55" s="20">
         <v>48</v>
       </c>
@@ -9438,7 +9441,7 @@
         <v>137</v>
       </c>
       <c r="P55" s="37" t="s">
-        <v>872</v>
+        <v>892</v>
       </c>
       <c r="Q55" s="25"/>
       <c r="R55" s="26" t="s">
@@ -12787,7 +12790,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="154" spans="1:20" ht="14.25" customHeight="1">
+    <row r="154" spans="1:20" ht="14.25" hidden="1" customHeight="1">
       <c r="A154" s="20">
         <v>147</v>
       </c>
@@ -12807,13 +12810,13 @@
         <v>45314</v>
       </c>
       <c r="G154" s="24" t="s">
+        <v>872</v>
+      </c>
+      <c r="H154" s="38" t="s">
         <v>873</v>
       </c>
-      <c r="H154" s="38" t="s">
+      <c r="I154" s="38" t="s">
         <v>874</v>
-      </c>
-      <c r="I154" s="38" t="s">
-        <v>875</v>
       </c>
       <c r="J154" s="25" t="s">
         <v>137</v>
@@ -13003,13 +13006,13 @@
         <v>45314</v>
       </c>
       <c r="G159" s="24" t="s">
+        <v>875</v>
+      </c>
+      <c r="H159" s="24" t="s">
         <v>876</v>
       </c>
-      <c r="H159" s="24" t="s">
+      <c r="I159" s="24" t="s">
         <v>877</v>
-      </c>
-      <c r="I159" s="24" t="s">
-        <v>878</v>
       </c>
       <c r="J159" s="25" t="s">
         <v>137</v>
@@ -13022,13 +13025,13 @@
         <v>137</v>
       </c>
       <c r="N159" s="37" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
       <c r="O159" s="25" t="s">
         <v>137</v>
       </c>
       <c r="P159" s="25" t="s">
-        <v>865</v>
+        <v>893</v>
       </c>
       <c r="Q159" s="25"/>
       <c r="R159" s="26"/>
@@ -13099,7 +13102,7 @@
         <v>825</v>
       </c>
       <c r="K161" s="37" t="s">
-        <v>880</v>
+        <v>879</v>
       </c>
       <c r="L161" s="25"/>
       <c r="M161" s="25"/>
@@ -13323,13 +13326,13 @@
         <v>45314</v>
       </c>
       <c r="G167" s="24" t="s">
+        <v>880</v>
+      </c>
+      <c r="H167" s="24" t="s">
         <v>881</v>
       </c>
-      <c r="H167" s="24" t="s">
+      <c r="I167" s="24" t="s">
         <v>882</v>
-      </c>
-      <c r="I167" s="24" t="s">
-        <v>883</v>
       </c>
       <c r="J167" s="25" t="s">
         <v>137</v>
@@ -13342,13 +13345,13 @@
         <v>137</v>
       </c>
       <c r="N167" s="37" t="s">
-        <v>884</v>
+        <v>883</v>
       </c>
       <c r="O167" s="37" t="s">
         <v>137</v>
       </c>
       <c r="P167" s="25" t="s">
-        <v>865</v>
+        <v>893</v>
       </c>
       <c r="Q167" s="25"/>
       <c r="R167" s="26"/>
@@ -13381,7 +13384,7 @@
         <v>825</v>
       </c>
       <c r="K168" s="37" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
       <c r="L168" s="25"/>
       <c r="M168" s="25"/>
@@ -13453,13 +13456,13 @@
         <v>45314</v>
       </c>
       <c r="G170" s="24" t="s">
+        <v>885</v>
+      </c>
+      <c r="H170" s="24" t="s">
         <v>886</v>
       </c>
-      <c r="H170" s="24" t="s">
+      <c r="I170" s="24" t="s">
         <v>887</v>
-      </c>
-      <c r="I170" s="24" t="s">
-        <v>888</v>
       </c>
       <c r="J170" s="25" t="s">
         <v>137</v>
@@ -13472,13 +13475,13 @@
         <v>137</v>
       </c>
       <c r="N170" s="37" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
       <c r="O170" s="37" t="s">
         <v>137</v>
       </c>
       <c r="P170" s="25" t="s">
-        <v>865</v>
+        <v>893</v>
       </c>
       <c r="Q170" s="25"/>
       <c r="R170" s="26"/>
@@ -20651,7 +20654,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="381" spans="1:20" ht="14.25" customHeight="1">
+    <row r="381" spans="1:20" ht="14.25" hidden="1" customHeight="1">
       <c r="A381" s="20">
         <v>374</v>
       </c>
@@ -20671,13 +20674,13 @@
         <v>45314</v>
       </c>
       <c r="G381" s="24" t="s">
+        <v>889</v>
+      </c>
+      <c r="H381" s="24" t="s">
         <v>890</v>
       </c>
-      <c r="H381" s="24" t="s">
+      <c r="I381" s="38" t="s">
         <v>891</v>
-      </c>
-      <c r="I381" s="38" t="s">
-        <v>892</v>
       </c>
       <c r="J381" s="25" t="s">
         <v>137</v>
@@ -25416,6 +25419,14 @@
     </row>
   </sheetData>
   <autoFilter ref="A9:T383" xr:uid="{00000000-0009-0000-0000-000002000000}">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="152"/>
+        <filter val="160"/>
+        <filter val="163"/>
+        <filter val="48"/>
+      </filters>
+    </filterColumn>
     <filterColumn colId="1">
       <filters>
         <filter val="VALIDAZIONE"/>
@@ -25425,11 +25436,6 @@
       <filters>
         <filter val="RSA"/>
       </filters>
-    </filterColumn>
-    <filterColumn colId="6">
-      <customFilters>
-        <customFilter operator="notEqual" val=" "/>
-      </customFilters>
     </filterColumn>
   </autoFilter>
   <mergeCells count="7">

</xml_diff>